<commit_message>
Início das tarefas apontadas na board.
</commit_message>
<xml_diff>
--- a/Board.xlsx
+++ b/Board.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osori\Documents\ISEP\Unidades Curriculares\1º Ano\2º Semestre\LAPR2\4 última semanas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ana\Dropbox\ISEP\2ºSemestre\LAPR2\Código-LAPR2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>Tarefas</t>
+  </si>
+  <si>
+    <t>Atribuído a:</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Problemas</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Relatório</t>
+  </si>
+  <si>
+    <t>Projeto</t>
+  </si>
+  <si>
+    <t>Análise do enunciado.</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Análise dos comentários relativos ao ultimo trabalho entregue nesta unicade curricular.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,19 +71,100 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -54,8 +173,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -71,6 +236,74 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3164851</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>159835</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2814297" cy="937629"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3774451" y="159835"/>
+          <a:ext cx="2814297" cy="937629"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="5400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Grupo 29</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -149,6 +382,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -184,6 +434,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -336,12 +603,315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="9">
+        <v>42520</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="9">
+        <v>42520</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:A18"/>
+    <mergeCell ref="A20:A35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização da board - divisão das tarefas relativas ao relatório.
</commit_message>
<xml_diff>
--- a/Board.xlsx
+++ b/Board.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osori\Documents\ISEP\Unidades Curriculares\1º Ano\2º Semestre\LAPR2\4 última semanas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ana\Dropbox\ISEP\2ºSemestre\LAPR2\codigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Tarefas</t>
   </si>
@@ -69,6 +69,48 @@
   </si>
   <si>
     <t>Ana Leite</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Introdução</t>
+  </si>
+  <si>
+    <t>State-of-the-art</t>
+  </si>
+  <si>
+    <t>Problema</t>
+  </si>
+  <si>
+    <t>Solução</t>
+  </si>
+  <si>
+    <t>Conclusão</t>
+  </si>
+  <si>
+    <t>Referencias</t>
+  </si>
+  <si>
+    <t>Revisão Ortográfica</t>
+  </si>
+  <si>
+    <t>Revisão da Organização</t>
+  </si>
+  <si>
+    <t>João Cardoso</t>
+  </si>
+  <si>
+    <t>Guilherme Ferreira</t>
+  </si>
+  <si>
+    <t>Ricardo Catalão</t>
+  </si>
+  <si>
+    <t>João Cardoso e Ricardo Catalão</t>
+  </si>
+  <si>
+    <t>Ana Leite e Guilherme Ferreira</t>
   </si>
 </sst>
 </file>
@@ -400,6 +442,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -435,6 +494,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -589,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,72 +723,108 @@
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="8"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="8"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="8"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="8"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="8"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="8"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="8"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="8"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="D15" s="6"/>
       <c r="E15" s="8"/>
       <c r="F15" s="2"/>

</xml_diff>

<commit_message>
Implementação do código aproveitável do trabalho de PPROG - Sem as correções
</commit_message>
<xml_diff>
--- a/Board.xlsx
+++ b/Board.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Tarefas</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Ana Leite</t>
+  </si>
+  <si>
+    <t>João Cardoso</t>
+  </si>
+  <si>
+    <t>Realização da documentação (Requisitos - formato breve) dos UC Remover candidaturaa exposição e Remover candidatura demonstração</t>
   </si>
 </sst>
 </file>
@@ -589,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="13" t="s">
         <v>12</v>
@@ -795,10 +801,14 @@
       <c r="E22" s="8"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="6"/>
+      <c r="B23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="D23" s="6"/>
       <c r="E23" s="8"/>
       <c r="F23" s="2"/>

</xml_diff>